<commit_message>
Casi todos los plots hechos
</commit_message>
<xml_diff>
--- a/metrics visualization/model_tests.xlsx
+++ b/metrics visualization/model_tests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="106">
   <si>
     <t>Divider</t>
   </si>
@@ -1233,7 +1233,7 @@
     <col min="16" max="16" style="79" width="15.43357142857143" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="80" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="2" width="83.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="2" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="2" width="596.4335714285714" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="22" max="22" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -3602,7 +3602,9 @@
         <f>MIN(VALUE(_xlfn.TEXTSPLIT(MID(S13, 2, LEN(S13) - 2), ",", TRUE)))</f>
       </c>
       <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
+      <c r="S13" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>

</xml_diff>